<commit_message>
Improving logging for run_model().
</commit_message>
<xml_diff>
--- a/tests/integration/integrated_models/1_coupled_model/concept.xlsx
+++ b/tests/integration/integrated_models/1_coupled_model/concept.xlsx
@@ -1,98 +1,74 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27531"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="27628"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\models\5 - coupled_model\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\git_repos\pyesm\tests\integration\integrated_models\1_coupled_model\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62520A7D-FF90-4B0A-A501-E685454A2864}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD8963FD-9AAC-4E78-BC48-AF488C3AC307}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-38490" yWindow="0" windowWidth="19380" windowHeight="20970" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-37640" yWindow="760" windowWidth="28800" windowHeight="15370" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="1" sheetId="1" r:id="rId1"/>
     <sheet name="2" sheetId="2" r:id="rId2"/>
-    <sheet name="2 (2)" sheetId="3" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="0" hidden="1">Gurobi</definedName>
     <definedName name="OpenSolver_ChosenSolver" localSheetId="1" hidden="1">CBC</definedName>
-    <definedName name="OpenSolver_ChosenSolver" localSheetId="2" hidden="1">CBC</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="0" hidden="1">0</definedName>
     <definedName name="OpenSolver_DualsNewSheet" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="OpenSolver_DualsNewSheet" localSheetId="2" hidden="1">0</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_LinearityCheck" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="OpenSolver_LinearityCheck" localSheetId="2" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="0" hidden="1">1</definedName>
     <definedName name="OpenSolver_UpdateSensitivity" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="OpenSolver_UpdateSensitivity" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_adj" localSheetId="0" hidden="1">'1'!$E$4:$F$4</definedName>
     <definedName name="solver_adj" localSheetId="1" hidden="1">'2'!$E$4:$F$4</definedName>
-    <definedName name="solver_adj" localSheetId="2" hidden="1">'2 (2)'!$E$5:$F$5</definedName>
     <definedName name="solver_cvg" localSheetId="0" hidden="1">0.0001</definedName>
     <definedName name="solver_cvg" localSheetId="1" hidden="1">0.0001</definedName>
-    <definedName name="solver_cvg" localSheetId="2" hidden="1">0.0001</definedName>
     <definedName name="solver_drv" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_drv" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_drv" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_est" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_est" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_itr" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_itr" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_itr" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_lhs1" localSheetId="0" hidden="1">'1'!$D$11</definedName>
     <definedName name="solver_lhs1" localSheetId="1" hidden="1">'2'!$E$11:$F$11</definedName>
-    <definedName name="solver_lhs1" localSheetId="2" hidden="1">'2 (2)'!$E$11:$F$11</definedName>
     <definedName name="solver_lhs2" localSheetId="0" hidden="1">'1'!$E$4:$F$4</definedName>
     <definedName name="solver_lhs3" localSheetId="0" hidden="1">'1'!$F$3</definedName>
     <definedName name="solver_neg" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_neg" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_neg" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_num" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_num" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_num" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_nwt" localSheetId="1" hidden="1">1</definedName>
-    <definedName name="solver_nwt" localSheetId="2" hidden="1">1</definedName>
     <definedName name="solver_opt" localSheetId="0" hidden="1">'1'!$D$10</definedName>
     <definedName name="solver_opt" localSheetId="1" hidden="1">'2'!$D$10</definedName>
-    <definedName name="solver_opt" localSheetId="2" hidden="1">'2 (2)'!$D$10</definedName>
     <definedName name="solver_rel1" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_rel1" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rel1" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_rel2" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rel3" localSheetId="0" hidden="1">3</definedName>
     <definedName name="solver_rhs1" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs1" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_rhs1" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_rhs2" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_rhs3" localSheetId="0" hidden="1">'1'!$H$3</definedName>
     <definedName name="solver_rlx" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_rlx" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_rlx" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="0" hidden="1">2</definedName>
     <definedName name="solver_scl" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_scl" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_sho" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_sho" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_sho" localSheetId="2" hidden="1">0</definedName>
     <definedName name="solver_tim" localSheetId="0" hidden="1">2147483647</definedName>
     <definedName name="solver_tim" localSheetId="1" hidden="1">2147483647</definedName>
-    <definedName name="solver_tim" localSheetId="2" hidden="1">2147483647</definedName>
     <definedName name="solver_tol" localSheetId="0" hidden="1">0.05</definedName>
     <definedName name="solver_tol" localSheetId="1" hidden="1">0.05</definedName>
-    <definedName name="solver_tol" localSheetId="2" hidden="1">0.05</definedName>
     <definedName name="solver_typ" localSheetId="0" hidden="1">1</definedName>
     <definedName name="solver_typ" localSheetId="1" hidden="1">2</definedName>
-    <definedName name="solver_typ" localSheetId="2" hidden="1">2</definedName>
     <definedName name="solver_val" localSheetId="0" hidden="1">0</definedName>
     <definedName name="solver_val" localSheetId="1" hidden="1">0</definedName>
-    <definedName name="solver_val" localSheetId="2" hidden="1">0</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -115,7 +91,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="107" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="72" uniqueCount="41">
   <si>
     <t>a</t>
   </si>
@@ -594,7 +570,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I12"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
+    <sheetView zoomScale="160" zoomScaleNormal="160" workbookViewId="0">
       <selection activeCell="E4" sqref="E4:F6"/>
     </sheetView>
   </sheetViews>
@@ -776,7 +752,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5E1A5120-BA3A-4F72-9BE3-44BB5F6207EF}">
   <dimension ref="A1:H33"/>
   <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="F5" sqref="F5"/>
     </sheetView>
   </sheetViews>
@@ -1166,400 +1142,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F480796D-6E03-4384-9FF1-958C6DF65CB7}">
-  <dimension ref="A1:H33"/>
-  <sheetViews>
-    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
-  <cols>
-    <col min="1" max="1" width="19.6328125" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" customWidth="1"/>
-    <col min="3" max="4" width="7.08984375" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A3" s="1" t="s">
-        <v>10</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>11</v>
-      </c>
-      <c r="C3" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="D3" s="1" t="s">
-        <v>8</v>
-      </c>
-      <c r="E3" s="1" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="1" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>27</v>
-      </c>
-      <c r="B4" t="s">
-        <v>12</v>
-      </c>
-      <c r="C4" t="s">
-        <v>0</v>
-      </c>
-      <c r="D4" t="s">
-        <v>23</v>
-      </c>
-      <c r="E4" s="4">
-        <v>0</v>
-      </c>
-      <c r="F4" s="4">
-        <v>0</v>
-      </c>
-      <c r="H4" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>9</v>
-      </c>
-      <c r="B5" t="s">
-        <v>16</v>
-      </c>
-      <c r="C5" t="s">
-        <v>6</v>
-      </c>
-      <c r="D5" t="s">
-        <v>2</v>
-      </c>
-      <c r="E5" s="7">
-        <v>1</v>
-      </c>
-      <c r="F5" s="7">
-        <v>10</v>
-      </c>
-      <c r="H5" t="s">
-        <v>38</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>31</v>
-      </c>
-      <c r="B6" t="s">
-        <v>16</v>
-      </c>
-      <c r="C6" t="s">
-        <v>32</v>
-      </c>
-      <c r="D6" t="s">
-        <v>23</v>
-      </c>
-      <c r="E6" s="3">
-        <v>0.9</v>
-      </c>
-      <c r="F6" s="3">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>33</v>
-      </c>
-      <c r="B7" t="s">
-        <v>16</v>
-      </c>
-      <c r="C7" t="s">
-        <v>34</v>
-      </c>
-      <c r="D7" t="s">
-        <v>23</v>
-      </c>
-      <c r="E7">
-        <v>-8.0000000000000002E-3</v>
-      </c>
-      <c r="F7">
-        <v>-2E-3</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>19</v>
-      </c>
-      <c r="C9" t="s">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>18</v>
-      </c>
-      <c r="B10" s="2" t="s">
-        <v>30</v>
-      </c>
-      <c r="D10">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>27</v>
-      </c>
-      <c r="B11" t="s">
-        <v>35</v>
-      </c>
-      <c r="C11" t="s">
-        <v>23</v>
-      </c>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3">
-        <f t="array" ref="E11:F11">E4:F4-E6:F6-E7:F7*E5:F5</f>
-        <v>-0.89200000000000002</v>
-      </c>
-      <c r="F11" s="3">
-        <v>-1.18</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D15" t="s">
-        <v>6</v>
-      </c>
-      <c r="E15" t="s">
-        <v>36</v>
-      </c>
-      <c r="F15" t="s">
-        <v>37</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="D16">
-        <v>0</v>
-      </c>
-      <c r="E16" s="3">
-        <f t="array" ref="E16:F16">$E$6:$F$6+$E$7:$F$7*D16</f>
-        <v>0.9</v>
-      </c>
-      <c r="F16" s="3">
-        <v>1.2</v>
-      </c>
-    </row>
-    <row r="17" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D17">
-        <v>5</v>
-      </c>
-      <c r="E17" s="3">
-        <f t="array" ref="E17:F17">$E$6:$F$6+$E$7:$F$7*D17</f>
-        <v>0.86</v>
-      </c>
-      <c r="F17" s="3">
-        <v>1.19</v>
-      </c>
-    </row>
-    <row r="18" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D18">
-        <v>10</v>
-      </c>
-      <c r="E18" s="3">
-        <f t="array" ref="E18:F18">$E$6:$F$6+$E$7:$F$7*D18</f>
-        <v>0.82000000000000006</v>
-      </c>
-      <c r="F18" s="3">
-        <v>1.18</v>
-      </c>
-    </row>
-    <row r="19" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D19">
-        <v>15</v>
-      </c>
-      <c r="E19" s="3">
-        <f t="array" ref="E19:F19">$E$6:$F$6+$E$7:$F$7*D19</f>
-        <v>0.78</v>
-      </c>
-      <c r="F19" s="3">
-        <v>1.17</v>
-      </c>
-    </row>
-    <row r="20" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D20">
-        <v>20</v>
-      </c>
-      <c r="E20" s="3">
-        <f t="array" ref="E20:F20">$E$6:$F$6+$E$7:$F$7*D20</f>
-        <v>0.74</v>
-      </c>
-      <c r="F20" s="3">
-        <v>1.1599999999999999</v>
-      </c>
-    </row>
-    <row r="21" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D21">
-        <v>25</v>
-      </c>
-      <c r="E21" s="3">
-        <f t="array" ref="E21:F21">$E$6:$F$6+$E$7:$F$7*D21</f>
-        <v>0.7</v>
-      </c>
-      <c r="F21" s="3">
-        <v>1.1499999999999999</v>
-      </c>
-    </row>
-    <row r="22" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D22">
-        <v>30</v>
-      </c>
-      <c r="E22" s="3">
-        <f t="array" ref="E22:F22">$E$6:$F$6+$E$7:$F$7*D22</f>
-        <v>0.66</v>
-      </c>
-      <c r="F22" s="3">
-        <v>1.1399999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D23">
-        <v>35</v>
-      </c>
-      <c r="E23" s="3">
-        <f t="array" ref="E23:F23">$E$6:$F$6+$E$7:$F$7*D23</f>
-        <v>0.62</v>
-      </c>
-      <c r="F23" s="3">
-        <v>1.1299999999999999</v>
-      </c>
-    </row>
-    <row r="24" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D24">
-        <v>40</v>
-      </c>
-      <c r="E24" s="3">
-        <f t="array" ref="E24:F24">$E$6:$F$6+$E$7:$F$7*D24</f>
-        <v>0.58000000000000007</v>
-      </c>
-      <c r="F24" s="3">
-        <v>1.1199999999999999</v>
-      </c>
-    </row>
-    <row r="25" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D25">
-        <v>45</v>
-      </c>
-      <c r="E25" s="3">
-        <f t="array" ref="E25:F25">$E$6:$F$6+$E$7:$F$7*D25</f>
-        <v>0.54</v>
-      </c>
-      <c r="F25" s="3">
-        <v>1.1099999999999999</v>
-      </c>
-    </row>
-    <row r="26" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D26">
-        <v>50</v>
-      </c>
-      <c r="E26" s="3">
-        <f t="array" ref="E26:F26">$E$6:$F$6+$E$7:$F$7*D26</f>
-        <v>0.5</v>
-      </c>
-      <c r="F26" s="3">
-        <v>1.0999999999999999</v>
-      </c>
-    </row>
-    <row r="27" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D27">
-        <v>55</v>
-      </c>
-      <c r="E27" s="3">
-        <f t="array" ref="E27:F27">$E$6:$F$6+$E$7:$F$7*D27</f>
-        <v>0.46</v>
-      </c>
-      <c r="F27" s="3">
-        <v>1.0899999999999999</v>
-      </c>
-    </row>
-    <row r="28" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D28">
-        <v>60</v>
-      </c>
-      <c r="E28" s="3">
-        <f t="array" ref="E28:F28">$E$6:$F$6+$E$7:$F$7*D28</f>
-        <v>0.42000000000000004</v>
-      </c>
-      <c r="F28" s="3">
-        <v>1.08</v>
-      </c>
-    </row>
-    <row r="29" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D29">
-        <v>65</v>
-      </c>
-      <c r="E29" s="3">
-        <f t="array" ref="E29:F29">$E$6:$F$6+$E$7:$F$7*D29</f>
-        <v>0.38</v>
-      </c>
-      <c r="F29" s="3">
-        <v>1.0699999999999998</v>
-      </c>
-    </row>
-    <row r="30" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D30">
-        <v>70</v>
-      </c>
-      <c r="E30" s="3">
-        <f t="array" ref="E30:F30">$E$6:$F$6+$E$7:$F$7*D30</f>
-        <v>0.33999999999999997</v>
-      </c>
-      <c r="F30" s="3">
-        <v>1.06</v>
-      </c>
-    </row>
-    <row r="31" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D31">
-        <v>75</v>
-      </c>
-      <c r="E31" s="3">
-        <f t="array" ref="E31:F31">$E$6:$F$6+$E$7:$F$7*D31</f>
-        <v>0.30000000000000004</v>
-      </c>
-      <c r="F31" s="3">
-        <v>1.05</v>
-      </c>
-    </row>
-    <row r="32" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D32">
-        <v>80</v>
-      </c>
-      <c r="E32" s="3">
-        <f t="array" ref="E32:F32">$E$6:$F$6+$E$7:$F$7*D32</f>
-        <v>0.26</v>
-      </c>
-      <c r="F32" s="3">
-        <v>1.04</v>
-      </c>
-    </row>
-    <row r="33" spans="4:6" x14ac:dyDescent="0.35">
-      <c r="D33">
-        <v>85</v>
-      </c>
-      <c r="E33" s="3">
-        <f t="array" ref="E33:F33">$E$6:$F$6+$E$7:$F$7*D33</f>
-        <v>0.21999999999999997</v>
-      </c>
-      <c r="F33" s="3">
-        <v>1.03</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>